<commit_message>
Parameterized version and Skip scenario implemented
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_7.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_7.xlsx
@@ -234,11 +234,35 @@
   <si>
     <t>Tags</t>
   </si>
+  <si>
+    <t>IncludesByPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@xml </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @ smoketest</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @smoketest</t>
+  </si>
+  <si>
+    <t>@pet @smoketest</t>
+  </si>
+  <si>
+    <t>@xml @smoketest</t>
+  </si>
+  <si>
+    <t>petId=id;petName=name;category_name=category.name</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="8" mc:Ignorable="x14ac">
   <numFmts count="8">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
@@ -249,7 +273,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="28">
     <font>
       <name val="Arial"/>
       <color rgb="FF000000"/>
@@ -309,8 +333,119 @@
       <sz val="12"/>
       <u val="single"/>
     </font>
+    <font>
+      <name val="Consolas"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <sz val="9"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Docs-Inconsolata"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Inconsolata"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="9"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Docs-Inconsolata"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Inconsolata"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Consolas"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="9"/>
+      <u val="single"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <u val="single"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,14 +458,41 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -347,6 +509,75 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,197 +802,214 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="topLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="18.53" customWidth="1"/>
     <col min="2" max="2" width="18.14" customWidth="1"/>
-    <col min="3" max="3" width="176.14" customWidth="1"/>
-    <col min="7" max="7" width="23.29" customWidth="1"/>
-    <col min="11" max="11" width="49.29" customWidth="1"/>
+    <col min="3" max="3" width="65.64" customWidth="1"/>
+    <col min="4" max="4" width="24.38" customWidth="1"/>
+    <col min="5" max="5" width="19.71" customWidth="1"/>
+    <col min="6" max="6" width="20.26" customWidth="1"/>
+    <col min="7" max="7" width="29.59" customWidth="1"/>
+    <col min="11" max="11" width="62.83" customWidth="1"/>
     <col min="12" max="12" width="24.29" customWidth="1"/>
     <col min="14" max="14" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="38" customFormat="1">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>15</v>
+      <c r="N1" s="50" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="3" t="s">
+    <row r="2" s="38" customFormat="1">
+      <c r="A2" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="43">
         <v>200</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="46"/>
+      <c r="L2" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="M2" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="46"/>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
+    <row r="3" s="38" customFormat="1">
+      <c r="A3" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="46"/>
+      <c r="F3" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="46"/>
+      <c r="H3" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="1">
+      <c r="I3" s="46"/>
+      <c r="J3" s="43">
         <v>200</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="7" t="s">
+      <c r="K3" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="46"/>
+      <c r="M3" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="N3" s="49" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
+    <row r="4" s="38" customFormat="1">
+      <c r="A4" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="G4" s="46"/>
+      <c r="H4" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="1">
+      <c r="I4" s="46"/>
+      <c r="J4" s="43">
         <v>200</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="K4" s="46"/>
+      <c r="L4" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="M4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="8" t="s">
+      <c r="M4" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
+    <row ht="13.5" customHeight="1" r="5" s="38" customFormat="1">
+      <c r="A5" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="G5" s="46"/>
+      <c r="H5" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="1">
+      <c r="I5" s="46"/>
+      <c r="J5" s="43">
         <v>200</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N5" t="s">
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" s="46" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>